<commit_message>
- Aider: corrections pour les importations de La Sarraz.
git-svn-id: https://svn.opac.ch/svn/cr/branches/vs2010.1@23323 787ff09c-d2b5-7842-b444-8dd0a418631d
</commit_message>
<xml_diff>
--- a/Epsitec.Cresus/App.Aider/Samples/La Sarraz/00.xlsx
+++ b/Epsitec.Cresus/App.Aider/Samples/La Sarraz/00.xlsx
@@ -20,7 +20,7 @@
     <definedName name="StartAider" localSheetId="0">[1]!Tableau1[[#Headers],[Num_AV]]</definedName>
     <definedName name="StartAider">[1]!Tableau1[[#Headers],[Num_AV]]</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="145621"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="844" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="239">
   <si>
     <t>ID Ménage</t>
   </si>
@@ -203,9 +203,6 @@
     <t>Cugny</t>
   </si>
   <si>
-    <t>Italie</t>
-  </si>
-  <si>
     <t>Nathalie</t>
   </si>
   <si>
@@ -605,9 +602,6 @@
     <t>Rue de l'Eglise</t>
   </si>
   <si>
-    <t>Yougoslavie</t>
-  </si>
-  <si>
     <t>021 861 32 25</t>
   </si>
   <si>
@@ -747,6 +741,12 @@
   </si>
   <si>
     <t>frd@loca-service.ch</t>
+  </si>
+  <si>
+    <t>IT</t>
+  </si>
+  <si>
+    <t>CH</t>
   </si>
 </sst>
 </file>
@@ -1098,7 +1098,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1112,7 +1112,7 @@
   <dimension ref="A1:AJ49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="S16" sqref="S16"/>
+      <selection activeCell="P38" sqref="P38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1228,19 +1228,19 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B2" t="s">
         <v>23</v>
       </c>
       <c r="C2" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="E2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G2" s="1">
         <v>17489</v>
@@ -1249,10 +1249,10 @@
         <v>24</v>
       </c>
       <c r="I2" t="s">
+        <v>86</v>
+      </c>
+      <c r="J2" t="s">
         <v>87</v>
-      </c>
-      <c r="J2" t="s">
-        <v>88</v>
       </c>
       <c r="L2">
         <v>1312</v>
@@ -1266,8 +1266,11 @@
       <c r="O2" t="s">
         <v>27</v>
       </c>
+      <c r="P2" t="s">
+        <v>238</v>
+      </c>
       <c r="Q2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="R2" t="s">
         <v>28</v>
@@ -1281,19 +1284,19 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="E3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G3" s="1">
         <v>20174</v>
@@ -1302,7 +1305,7 @@
         <v>24</v>
       </c>
       <c r="I3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="J3">
         <v>2</v>
@@ -1343,19 +1346,19 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
         <v>30</v>
       </c>
       <c r="C4" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F4" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G4" s="1">
         <v>27758</v>
@@ -1364,7 +1367,7 @@
         <v>24</v>
       </c>
       <c r="I4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J4">
         <v>2</v>
@@ -1381,8 +1384,11 @@
       <c r="O4" t="s">
         <v>31</v>
       </c>
+      <c r="P4" t="s">
+        <v>238</v>
+      </c>
       <c r="Q4" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R4" t="s">
         <v>28</v>
@@ -1391,7 +1397,7 @@
         <v>24</v>
       </c>
       <c r="T4" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U4" t="s">
         <v>24</v>
@@ -1405,19 +1411,19 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B5" t="s">
         <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G5" s="1">
         <v>39347</v>
@@ -1426,7 +1432,7 @@
         <v>24</v>
       </c>
       <c r="I5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J5">
         <v>2</v>
@@ -1443,8 +1449,11 @@
       <c r="O5" t="s">
         <v>27</v>
       </c>
+      <c r="P5" t="s">
+        <v>238</v>
+      </c>
       <c r="Q5" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R5" t="s">
         <v>36</v>
@@ -1453,7 +1462,7 @@
         <v>24</v>
       </c>
       <c r="T5" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U5" t="s">
         <v>24</v>
@@ -1467,19 +1476,19 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B6" t="s">
         <v>39</v>
       </c>
       <c r="C6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="F6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G6" s="1">
         <v>40285</v>
@@ -1488,7 +1497,7 @@
         <v>24</v>
       </c>
       <c r="I6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J6">
         <v>2</v>
@@ -1505,8 +1514,11 @@
       <c r="O6" t="s">
         <v>31</v>
       </c>
+      <c r="P6" t="s">
+        <v>238</v>
+      </c>
       <c r="Q6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="R6" t="s">
         <v>36</v>
@@ -1515,7 +1527,7 @@
         <v>24</v>
       </c>
       <c r="T6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="U6" t="s">
         <v>24</v>
@@ -1529,13 +1541,13 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B7" t="s">
         <v>23</v>
       </c>
       <c r="C7" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E7" t="s">
         <v>51</v>
@@ -1550,10 +1562,10 @@
         <v>24</v>
       </c>
       <c r="I7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="L7">
         <v>1315</v>
@@ -1567,14 +1579,14 @@
       <c r="O7" t="s">
         <v>27</v>
       </c>
-      <c r="Q7" t="s">
-        <v>57</v>
+      <c r="P7" t="s">
+        <v>237</v>
       </c>
       <c r="R7" t="s">
         <v>28</v>
       </c>
       <c r="S7" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="T7" t="s">
         <v>24</v>
@@ -1591,19 +1603,19 @@
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B8" t="s">
         <v>23</v>
       </c>
       <c r="C8" t="s">
+        <v>102</v>
+      </c>
+      <c r="E8" t="s">
         <v>103</v>
       </c>
-      <c r="E8" t="s">
-        <v>104</v>
-      </c>
       <c r="F8" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G8" s="1">
         <v>26995</v>
@@ -1612,7 +1624,7 @@
         <v>24</v>
       </c>
       <c r="I8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="J8" t="s">
         <v>53</v>
@@ -1639,7 +1651,7 @@
         <v>24</v>
       </c>
       <c r="T8" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="U8" t="s">
         <v>24</v>
@@ -1653,19 +1665,19 @@
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B9" t="s">
         <v>30</v>
       </c>
       <c r="C9" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" t="s">
         <v>108</v>
       </c>
-      <c r="E9" t="s">
-        <v>109</v>
-      </c>
       <c r="F9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="G9" s="1">
         <v>13113</v>
@@ -1674,7 +1686,7 @@
         <v>24</v>
       </c>
       <c r="I9" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J9">
         <v>6</v>
@@ -1695,13 +1707,13 @@
         <v>24</v>
       </c>
       <c r="R9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S9" t="s">
         <v>24</v>
       </c>
       <c r="T9" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="W9" t="s">
         <v>24</v>
@@ -1709,7 +1721,7 @@
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B10" t="s">
         <v>23</v>
@@ -1718,16 +1730,16 @@
         <v>43</v>
       </c>
       <c r="E10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="F10" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="G10" s="1">
         <v>27062</v>
       </c>
       <c r="H10" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="I10" t="s">
         <v>29</v>
@@ -1747,11 +1759,14 @@
       <c r="O10" t="s">
         <v>27</v>
       </c>
+      <c r="P10" t="s">
+        <v>238</v>
+      </c>
       <c r="Q10" t="s">
         <v>44</v>
       </c>
       <c r="S10" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="T10" t="s">
         <v>24</v>
@@ -1768,7 +1783,7 @@
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B11" t="s">
         <v>23</v>
@@ -1777,10 +1792,10 @@
         <v>43</v>
       </c>
       <c r="E11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F11" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G11" s="1">
         <v>35721</v>
@@ -1806,6 +1821,9 @@
       <c r="O11" t="s">
         <v>27</v>
       </c>
+      <c r="P11" t="s">
+        <v>238</v>
+      </c>
       <c r="Q11" t="s">
         <v>44</v>
       </c>
@@ -1813,7 +1831,7 @@
         <v>36</v>
       </c>
       <c r="S11" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="T11" t="s">
         <v>24</v>
@@ -1830,7 +1848,7 @@
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B12" t="s">
         <v>23</v>
@@ -1875,7 +1893,7 @@
         <v>36</v>
       </c>
       <c r="S12" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="T12" t="s">
         <v>24</v>
@@ -1892,19 +1910,19 @@
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B13" t="s">
         <v>23</v>
       </c>
       <c r="C13" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G13" s="1">
         <v>30933</v>
@@ -1913,7 +1931,7 @@
         <v>24</v>
       </c>
       <c r="I13" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J13">
         <v>7</v>
@@ -1951,25 +1969,25 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B14" t="s">
         <v>30</v>
       </c>
       <c r="C14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="F14" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="H14" t="s">
         <v>24</v>
       </c>
       <c r="I14" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="J14">
         <v>3</v>
@@ -1993,16 +2011,16 @@
         <v>28</v>
       </c>
       <c r="S14" t="s">
+        <v>123</v>
+      </c>
+      <c r="T14" t="s">
         <v>124</v>
       </c>
-      <c r="T14" t="s">
+      <c r="U14" t="s">
+        <v>24</v>
+      </c>
+      <c r="V14" t="s">
         <v>125</v>
-      </c>
-      <c r="U14" t="s">
-        <v>24</v>
-      </c>
-      <c r="V14" t="s">
-        <v>126</v>
       </c>
       <c r="W14" t="s">
         <v>24</v>
@@ -2010,19 +2028,19 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B15" t="s">
         <v>30</v>
       </c>
       <c r="C15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G15" s="1">
         <v>24261</v>
@@ -2031,7 +2049,7 @@
         <v>24</v>
       </c>
       <c r="I15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J15">
         <v>8</v>
@@ -2048,17 +2066,20 @@
       <c r="O15" t="s">
         <v>31</v>
       </c>
+      <c r="P15" t="s">
+        <v>238</v>
+      </c>
       <c r="Q15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="R15" t="s">
         <v>37</v>
       </c>
       <c r="S15" t="s">
+        <v>129</v>
+      </c>
+      <c r="T15" t="s">
         <v>130</v>
-      </c>
-      <c r="T15" t="s">
-        <v>131</v>
       </c>
       <c r="W15" t="s">
         <v>24</v>
@@ -2066,19 +2087,19 @@
     </row>
     <row r="16" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
         <v>30</v>
       </c>
       <c r="C16" t="s">
+        <v>132</v>
+      </c>
+      <c r="E16" t="s">
         <v>133</v>
       </c>
-      <c r="E16" t="s">
-        <v>134</v>
-      </c>
       <c r="F16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G16" s="1">
         <v>38730</v>
@@ -2087,7 +2108,7 @@
         <v>24</v>
       </c>
       <c r="I16" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J16" t="s">
         <v>47</v>
@@ -2114,13 +2135,13 @@
         <v>24</v>
       </c>
       <c r="T16" t="s">
+        <v>134</v>
+      </c>
+      <c r="U16" t="s">
+        <v>24</v>
+      </c>
+      <c r="V16" t="s">
         <v>135</v>
-      </c>
-      <c r="U16" t="s">
-        <v>24</v>
-      </c>
-      <c r="V16" t="s">
-        <v>136</v>
       </c>
       <c r="W16" t="s">
         <v>24</v>
@@ -2128,19 +2149,19 @@
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B17" t="s">
         <v>23</v>
       </c>
       <c r="C17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="F17" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G17" s="1">
         <v>38730</v>
@@ -2149,7 +2170,7 @@
         <v>24</v>
       </c>
       <c r="I17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J17" t="s">
         <v>47</v>
@@ -2176,27 +2197,27 @@
         <v>24</v>
       </c>
       <c r="T17" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="U17" t="s">
         <v>24</v>
       </c>
       <c r="V17" t="s">
+        <v>137</v>
+      </c>
+      <c r="W17" t="s">
         <v>138</v>
-      </c>
-      <c r="W17" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B18" t="s">
         <v>23</v>
       </c>
       <c r="C18" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E18" t="s">
         <v>54</v>
@@ -2211,7 +2232,7 @@
         <v>24</v>
       </c>
       <c r="I18" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="J18" t="s">
         <v>47</v>
@@ -2238,27 +2259,27 @@
         <v>24</v>
       </c>
       <c r="T18" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="U18" t="s">
         <v>24</v>
       </c>
       <c r="V18" t="s">
+        <v>137</v>
+      </c>
+      <c r="W18" t="s">
         <v>138</v>
-      </c>
-      <c r="W18" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B19" t="s">
         <v>30</v>
       </c>
       <c r="C19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E19" t="s">
         <v>55</v>
@@ -2270,10 +2291,10 @@
         <v>24</v>
       </c>
       <c r="I19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J19" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L19">
         <v>1315</v>
@@ -2297,7 +2318,7 @@
         <v>24</v>
       </c>
       <c r="T19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="U19" t="s">
         <v>24</v>
@@ -2311,19 +2332,19 @@
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B20" t="s">
         <v>23</v>
       </c>
       <c r="C20" t="s">
+        <v>144</v>
+      </c>
+      <c r="E20" t="s">
         <v>145</v>
       </c>
-      <c r="E20" t="s">
-        <v>146</v>
-      </c>
       <c r="F20" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G20" s="1">
         <v>25806</v>
@@ -2332,7 +2353,7 @@
         <v>24</v>
       </c>
       <c r="I20" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -2349,8 +2370,8 @@
       <c r="O20" t="s">
         <v>27</v>
       </c>
-      <c r="Q20" t="s">
-        <v>57</v>
+      <c r="P20" t="s">
+        <v>237</v>
       </c>
       <c r="R20" t="s">
         <v>28</v>
@@ -2359,33 +2380,33 @@
         <v>24</v>
       </c>
       <c r="T20" t="s">
+        <v>147</v>
+      </c>
+      <c r="U20" t="s">
+        <v>24</v>
+      </c>
+      <c r="V20" t="s">
+        <v>137</v>
+      </c>
+      <c r="W20" t="s">
         <v>148</v>
-      </c>
-      <c r="U20" t="s">
-        <v>24</v>
-      </c>
-      <c r="V20" t="s">
-        <v>138</v>
-      </c>
-      <c r="W20" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B21" t="s">
         <v>30</v>
       </c>
       <c r="C21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="F21" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G21" s="1">
         <v>27376</v>
@@ -2394,7 +2415,7 @@
         <v>24</v>
       </c>
       <c r="I21" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -2421,33 +2442,33 @@
         <v>24</v>
       </c>
       <c r="T21" t="s">
+        <v>147</v>
+      </c>
+      <c r="U21" t="s">
+        <v>24</v>
+      </c>
+      <c r="V21" t="s">
+        <v>24</v>
+      </c>
+      <c r="W21" t="s">
         <v>148</v>
-      </c>
-      <c r="U21" t="s">
-        <v>24</v>
-      </c>
-      <c r="V21" t="s">
-        <v>24</v>
-      </c>
-      <c r="W21" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B22" t="s">
         <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="F22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G22" s="1">
         <v>37505</v>
@@ -2456,7 +2477,7 @@
         <v>24</v>
       </c>
       <c r="I22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -2483,33 +2504,33 @@
         <v>24</v>
       </c>
       <c r="T22" t="s">
+        <v>147</v>
+      </c>
+      <c r="U22" t="s">
+        <v>24</v>
+      </c>
+      <c r="V22" t="s">
+        <v>24</v>
+      </c>
+      <c r="W22" t="s">
         <v>148</v>
-      </c>
-      <c r="U22" t="s">
-        <v>24</v>
-      </c>
-      <c r="V22" t="s">
-        <v>24</v>
-      </c>
-      <c r="W22" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B23" t="s">
         <v>23</v>
       </c>
       <c r="C23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="F23" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G23" s="1">
         <v>38641</v>
@@ -2518,7 +2539,7 @@
         <v>24</v>
       </c>
       <c r="I23" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -2545,33 +2566,33 @@
         <v>24</v>
       </c>
       <c r="T23" t="s">
+        <v>147</v>
+      </c>
+      <c r="U23" t="s">
+        <v>24</v>
+      </c>
+      <c r="V23" t="s">
+        <v>137</v>
+      </c>
+      <c r="W23" t="s">
         <v>148</v>
-      </c>
-      <c r="U23" t="s">
-        <v>24</v>
-      </c>
-      <c r="V23" t="s">
-        <v>138</v>
-      </c>
-      <c r="W23" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B24" t="s">
         <v>23</v>
       </c>
       <c r="C24" t="s">
+        <v>153</v>
+      </c>
+      <c r="E24" t="s">
         <v>154</v>
       </c>
-      <c r="E24" t="s">
-        <v>155</v>
-      </c>
       <c r="F24" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G24" s="1">
         <v>15424</v>
@@ -2580,7 +2601,7 @@
         <v>24</v>
       </c>
       <c r="I24" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J24" t="s">
         <v>50</v>
@@ -2597,8 +2618,11 @@
       <c r="O24" t="s">
         <v>27</v>
       </c>
+      <c r="P24" t="s">
+        <v>238</v>
+      </c>
       <c r="Q24" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R24" t="s">
         <v>37</v>
@@ -2621,25 +2645,25 @@
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B25" t="s">
         <v>30</v>
       </c>
       <c r="C25" t="s">
+        <v>157</v>
+      </c>
+      <c r="E25" t="s">
         <v>158</v>
       </c>
-      <c r="E25" t="s">
+      <c r="F25" t="s">
+        <v>158</v>
+      </c>
+      <c r="H25" t="s">
+        <v>24</v>
+      </c>
+      <c r="I25" t="s">
         <v>159</v>
-      </c>
-      <c r="F25" t="s">
-        <v>159</v>
-      </c>
-      <c r="H25" t="s">
-        <v>24</v>
-      </c>
-      <c r="I25" t="s">
-        <v>160</v>
       </c>
       <c r="J25">
         <v>5</v>
@@ -2666,7 +2690,7 @@
         <v>24</v>
       </c>
       <c r="T25" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="U25" t="s">
         <v>24</v>
@@ -2680,19 +2704,19 @@
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B26" t="s">
         <v>30</v>
       </c>
       <c r="C26" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F26" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G26" s="1">
         <v>18349</v>
@@ -2701,10 +2725,10 @@
         <v>24</v>
       </c>
       <c r="I26" t="s">
+        <v>163</v>
+      </c>
+      <c r="J26" t="s">
         <v>164</v>
-      </c>
-      <c r="J26" t="s">
-        <v>165</v>
       </c>
       <c r="L26">
         <v>1315</v>
@@ -2718,8 +2742,11 @@
       <c r="O26" t="s">
         <v>31</v>
       </c>
+      <c r="P26" t="s">
+        <v>238</v>
+      </c>
       <c r="Q26" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="R26" t="s">
         <v>37</v>
@@ -2742,28 +2769,28 @@
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B27" t="s">
         <v>30</v>
       </c>
       <c r="C27" t="s">
+        <v>167</v>
+      </c>
+      <c r="E27" t="s">
+        <v>57</v>
+      </c>
+      <c r="F27" t="s">
+        <v>57</v>
+      </c>
+      <c r="H27" t="s">
         <v>168</v>
       </c>
-      <c r="E27" t="s">
-        <v>58</v>
-      </c>
-      <c r="F27" t="s">
-        <v>58</v>
-      </c>
-      <c r="H27" t="s">
+      <c r="I27" t="s">
         <v>169</v>
       </c>
-      <c r="I27" t="s">
-        <v>170</v>
-      </c>
       <c r="J27" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L27">
         <v>1315</v>
@@ -2801,7 +2828,7 @@
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B28" t="s">
         <v>23</v>
@@ -2810,10 +2837,10 @@
         <v>56</v>
       </c>
       <c r="E28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F28" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G28" s="1">
         <v>18016</v>
@@ -2822,7 +2849,7 @@
         <v>24</v>
       </c>
       <c r="I28" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="J28">
         <v>1</v>
@@ -2860,19 +2887,19 @@
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B29" t="s">
         <v>23</v>
       </c>
       <c r="C29" t="s">
+        <v>174</v>
+      </c>
+      <c r="E29" t="s">
         <v>175</v>
       </c>
-      <c r="E29" t="s">
-        <v>176</v>
-      </c>
       <c r="F29" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G29" s="1">
         <v>39172</v>
@@ -2881,7 +2908,7 @@
         <v>24</v>
       </c>
       <c r="I29" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J29" t="s">
         <v>49</v>
@@ -2898,8 +2925,11 @@
       <c r="O29" t="s">
         <v>27</v>
       </c>
+      <c r="P29" t="s">
+        <v>238</v>
+      </c>
       <c r="Q29" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="R29" t="s">
         <v>36</v>
@@ -2913,25 +2943,25 @@
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B30" t="s">
         <v>30</v>
       </c>
       <c r="C30" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E30" t="s">
+        <v>179</v>
+      </c>
+      <c r="F30" t="s">
+        <v>179</v>
+      </c>
+      <c r="H30" t="s">
+        <v>24</v>
+      </c>
+      <c r="I30" t="s">
         <v>180</v>
-      </c>
-      <c r="F30" t="s">
-        <v>180</v>
-      </c>
-      <c r="H30" t="s">
-        <v>24</v>
-      </c>
-      <c r="I30" t="s">
-        <v>181</v>
       </c>
       <c r="J30">
         <v>3</v>
@@ -2969,13 +2999,13 @@
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B31" t="s">
         <v>23</v>
       </c>
       <c r="C31" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="E31" t="s">
         <v>48</v>
@@ -2987,10 +3017,10 @@
         <v>24</v>
       </c>
       <c r="I31" t="s">
+        <v>183</v>
+      </c>
+      <c r="J31" t="s">
         <v>184</v>
-      </c>
-      <c r="J31" t="s">
-        <v>185</v>
       </c>
       <c r="L31">
         <v>1317</v>
@@ -3014,7 +3044,7 @@
         <v>24</v>
       </c>
       <c r="T31" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="U31" t="s">
         <v>24</v>
@@ -3028,28 +3058,28 @@
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B32" t="s">
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G32" s="1">
         <v>22068</v>
       </c>
       <c r="H32" t="s">
+        <v>188</v>
+      </c>
+      <c r="I32" t="s">
         <v>189</v>
-      </c>
-      <c r="I32" t="s">
-        <v>190</v>
       </c>
       <c r="L32">
         <v>1316</v>
@@ -3063,17 +3093,14 @@
       <c r="O32" t="s">
         <v>27</v>
       </c>
-      <c r="Q32" t="s">
-        <v>191</v>
-      </c>
       <c r="R32" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S32" t="s">
         <v>24</v>
       </c>
       <c r="T32" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="W32" t="s">
         <v>24</v>
@@ -3081,19 +3108,19 @@
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B33" t="s">
         <v>39</v>
       </c>
       <c r="C33" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="E33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="F33" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="G33" s="1">
         <v>35427</v>
@@ -3102,7 +3129,7 @@
         <v>24</v>
       </c>
       <c r="I33" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L33">
         <v>1316</v>
@@ -3116,6 +3143,9 @@
       <c r="O33" t="s">
         <v>31</v>
       </c>
+      <c r="P33" t="s">
+        <v>238</v>
+      </c>
       <c r="Q33" t="s">
         <v>25</v>
       </c>
@@ -3126,7 +3156,7 @@
         <v>24</v>
       </c>
       <c r="T33" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="W33" t="s">
         <v>24</v>
@@ -3134,19 +3164,19 @@
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
       </c>
       <c r="C34" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E34" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="F34" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="G34" s="1">
         <v>26601</v>
@@ -3155,7 +3185,7 @@
         <v>24</v>
       </c>
       <c r="I34" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J34" t="s">
         <v>34</v>
@@ -3172,8 +3202,11 @@
       <c r="O34" t="s">
         <v>31</v>
       </c>
+      <c r="P34" t="s">
+        <v>238</v>
+      </c>
       <c r="Q34" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R34" t="s">
         <v>24</v>
@@ -3196,28 +3229,28 @@
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B35" t="s">
         <v>23</v>
       </c>
       <c r="C35" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F35" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G35" s="1">
         <v>26733</v>
       </c>
       <c r="H35" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="I35" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J35" t="s">
         <v>34</v>
@@ -3234,8 +3267,11 @@
       <c r="O35" t="s">
         <v>27</v>
       </c>
+      <c r="P35" t="s">
+        <v>238</v>
+      </c>
       <c r="Q35" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R35" t="s">
         <v>28</v>
@@ -3258,19 +3294,19 @@
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B36" t="s">
         <v>39</v>
       </c>
       <c r="C36" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F36" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="G36" s="1">
         <v>39148</v>
@@ -3279,7 +3315,7 @@
         <v>24</v>
       </c>
       <c r="I36" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J36" t="s">
         <v>34</v>
@@ -3296,8 +3332,11 @@
       <c r="O36" t="s">
         <v>31</v>
       </c>
+      <c r="P36" t="s">
+        <v>238</v>
+      </c>
       <c r="Q36" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R36" t="s">
         <v>36</v>
@@ -3320,19 +3359,19 @@
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B37" t="s">
         <v>39</v>
       </c>
       <c r="C37" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="E37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F37" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="G37" s="1">
         <v>39701</v>
@@ -3341,7 +3380,7 @@
         <v>24</v>
       </c>
       <c r="I37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="J37" t="s">
         <v>34</v>
@@ -3358,8 +3397,11 @@
       <c r="O37" t="s">
         <v>31</v>
       </c>
+      <c r="P37" t="s">
+        <v>238</v>
+      </c>
       <c r="Q37" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="R37" t="s">
         <v>36</v>
@@ -3382,28 +3424,28 @@
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="B38" t="s">
         <v>23</v>
       </c>
       <c r="C38" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="E38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="F38" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G38" s="1">
         <v>31232</v>
       </c>
       <c r="H38" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="I38" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J38" t="s">
         <v>34</v>
@@ -3420,8 +3462,11 @@
       <c r="O38" t="s">
         <v>27</v>
       </c>
+      <c r="P38" t="s">
+        <v>238</v>
+      </c>
       <c r="Q38" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="R38" t="s">
         <v>28</v>
@@ -3444,19 +3489,19 @@
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B39" t="s">
         <v>30</v>
       </c>
       <c r="C39" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="E39" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="F39" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G39" s="1">
         <v>25144</v>
@@ -3465,7 +3510,7 @@
         <v>24</v>
       </c>
       <c r="I39" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="J39" t="s">
         <v>49</v>
@@ -3486,7 +3531,7 @@
         <v>24</v>
       </c>
       <c r="S39" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="W39" t="s">
         <v>24</v>
@@ -3494,19 +3539,19 @@
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B40" t="s">
         <v>23</v>
       </c>
       <c r="C40" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="E40" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="F40" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G40" s="1">
         <v>14112</v>
@@ -3515,7 +3560,7 @@
         <v>24</v>
       </c>
       <c r="I40" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J40">
         <v>4</v>
@@ -3536,13 +3581,13 @@
         <v>24</v>
       </c>
       <c r="R40" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S40" t="s">
         <v>24</v>
       </c>
       <c r="T40" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="U40" t="s">
         <v>24</v>
@@ -3556,28 +3601,28 @@
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B41" t="s">
         <v>30</v>
       </c>
       <c r="C41" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="E41" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="F41" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="H41" t="s">
         <v>24</v>
       </c>
       <c r="I41" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="J41" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L41">
         <v>1315</v>
@@ -3601,7 +3646,7 @@
         <v>24</v>
       </c>
       <c r="T41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="U41" t="s">
         <v>24</v>
@@ -3615,28 +3660,28 @@
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B42" t="s">
         <v>23</v>
       </c>
       <c r="C42" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F42" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G42" s="1">
         <v>15674</v>
       </c>
       <c r="H42" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I42" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J42" t="s">
         <v>40</v>
@@ -3677,19 +3722,19 @@
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B43" t="s">
         <v>30</v>
       </c>
       <c r="C43" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E43" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="F43" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="G43" s="1">
         <v>17738</v>
@@ -3698,7 +3743,7 @@
         <v>24</v>
       </c>
       <c r="I43" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J43" t="s">
         <v>40</v>
@@ -3739,25 +3784,25 @@
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B44" t="s">
         <v>30</v>
       </c>
       <c r="C44" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="F44" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="H44" t="s">
         <v>24</v>
       </c>
       <c r="I44" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J44">
         <v>8</v>
@@ -3795,28 +3840,28 @@
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B45" t="s">
         <v>39</v>
       </c>
       <c r="C45" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E45" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="F45" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="H45" t="s">
         <v>24</v>
       </c>
       <c r="I45" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J45" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="L45">
         <v>1315</v>
@@ -3854,28 +3899,28 @@
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B46" t="s">
         <v>30</v>
       </c>
       <c r="C46" t="s">
+        <v>223</v>
+      </c>
+      <c r="E46" t="s">
+        <v>224</v>
+      </c>
+      <c r="F46" t="s">
+        <v>224</v>
+      </c>
+      <c r="H46" t="s">
+        <v>24</v>
+      </c>
+      <c r="I46" t="s">
         <v>225</v>
       </c>
-      <c r="E46" t="s">
-        <v>226</v>
-      </c>
-      <c r="F46" t="s">
-        <v>226</v>
-      </c>
-      <c r="H46" t="s">
-        <v>24</v>
-      </c>
-      <c r="I46" t="s">
-        <v>227</v>
-      </c>
       <c r="J46" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L46">
         <v>1313</v>
@@ -3913,28 +3958,28 @@
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B47" t="s">
         <v>23</v>
       </c>
       <c r="C47" t="s">
+        <v>223</v>
+      </c>
+      <c r="E47" t="s">
+        <v>226</v>
+      </c>
+      <c r="F47" t="s">
+        <v>226</v>
+      </c>
+      <c r="H47" t="s">
+        <v>24</v>
+      </c>
+      <c r="I47" t="s">
         <v>225</v>
       </c>
-      <c r="E47" t="s">
-        <v>228</v>
-      </c>
-      <c r="F47" t="s">
-        <v>228</v>
-      </c>
-      <c r="H47" t="s">
-        <v>24</v>
-      </c>
-      <c r="I47" t="s">
-        <v>227</v>
-      </c>
       <c r="J47" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L47">
         <v>1313</v>
@@ -3972,25 +4017,25 @@
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B48" t="s">
         <v>30</v>
       </c>
       <c r="C48" t="s">
+        <v>228</v>
+      </c>
+      <c r="E48" t="s">
+        <v>229</v>
+      </c>
+      <c r="F48" t="s">
+        <v>229</v>
+      </c>
+      <c r="H48" t="s">
+        <v>24</v>
+      </c>
+      <c r="I48" t="s">
         <v>230</v>
-      </c>
-      <c r="E48" t="s">
-        <v>231</v>
-      </c>
-      <c r="F48" t="s">
-        <v>231</v>
-      </c>
-      <c r="H48" t="s">
-        <v>24</v>
-      </c>
-      <c r="I48" t="s">
-        <v>232</v>
       </c>
       <c r="J48">
         <v>6</v>
@@ -4011,13 +4056,13 @@
         <v>24</v>
       </c>
       <c r="R48" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="S48" t="s">
         <v>24</v>
       </c>
       <c r="T48" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="U48" t="s">
         <v>24</v>
@@ -4031,19 +4076,19 @@
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B49" t="s">
         <v>39</v>
       </c>
       <c r="C49" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="E49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="F49" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G49" s="1">
         <v>38924</v>
@@ -4052,10 +4097,10 @@
         <v>24</v>
       </c>
       <c r="I49" t="s">
+        <v>183</v>
+      </c>
+      <c r="J49" t="s">
         <v>184</v>
-      </c>
-      <c r="J49" t="s">
-        <v>185</v>
       </c>
       <c r="L49">
         <v>1317</v>
@@ -4076,19 +4121,19 @@
         <v>36</v>
       </c>
       <c r="S49" t="s">
+        <v>234</v>
+      </c>
+      <c r="T49" t="s">
+        <v>185</v>
+      </c>
+      <c r="U49" t="s">
+        <v>24</v>
+      </c>
+      <c r="V49" t="s">
+        <v>235</v>
+      </c>
+      <c r="W49" t="s">
         <v>236</v>
-      </c>
-      <c r="T49" t="s">
-        <v>186</v>
-      </c>
-      <c r="U49" t="s">
-        <v>24</v>
-      </c>
-      <c r="V49" t="s">
-        <v>237</v>
-      </c>
-      <c r="W49" t="s">
-        <v>238</v>
       </c>
     </row>
   </sheetData>

</xml_diff>